<commit_message>
♻️ unify common code
</commit_message>
<xml_diff>
--- a/StochasticShortestPath_Static/Parameters.xlsx
+++ b/StochasticShortestPath_Static/Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnascime/Dropbox/PythonProjects/ORF411/github_private/seqdecisionlib_ShortestPath_Static/Stochastic_Shortest_Path_Static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeongjun-u/Documents/GitHub/optimization-theory/StochasticShortestPath_Static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ADB17F-37F4-DE4A-833C-20B1D8953E8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B45E9F-12FC-794E-B4C5-78323EB54C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="680" windowWidth="19620" windowHeight="10160" activeTab="1" xr2:uid="{0DB32CC8-A0F8-4A1F-8469-0451A56A93A9}"/>
+    <workbookView xWindow="13340" yWindow="-20320" windowWidth="19840" windowHeight="13240" activeTab="1" xr2:uid="{0DB32CC8-A0F8-4A1F-8469-0451A56A93A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="4" r:id="rId1"/>
@@ -43,9 +43,6 @@
     <t>Index</t>
   </si>
   <si>
-    <t>Constant</t>
-  </si>
-  <si>
     <t>stepsize_rule</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t>probEdge</t>
   </si>
   <si>
-    <t>1 .5 .2 .1</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Use sheet </t>
     </r>
@@ -66,7 +60,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -76,7 +70,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -101,7 +95,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -111,7 +105,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -122,7 +116,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -138,7 +132,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -148,7 +142,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -159,7 +153,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -169,7 +163,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -180,7 +174,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -190,7 +184,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -201,7 +195,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -213,7 +207,7 @@
         <i/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -223,23 +217,31 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> inside "StaticModelAdaptive.py"</t>
     </r>
+  </si>
+  <si>
+    <t>Declining</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 5 10 20 50</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -247,7 +249,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -256,8 +258,15 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -288,7 +297,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -304,9 +313,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -344,7 +353,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -450,7 +459,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -592,7 +601,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -602,46 +611,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BC70B3A-BEBA-564B-A9E3-005424252FEF}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="83.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="36">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="72">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="36">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="54">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="54">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -651,16 +661,16 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -668,23 +678,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -692,7 +702,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -700,7 +710,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -708,23 +718,24 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>